<commit_message>
added tab-delimited results file. removed references. updated user guide.
</commit_message>
<xml_diff>
--- a/www/DASSApp-dataTemplate.xlsx
+++ b/www/DASSApp-dataTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kto\Documents\repos\dass\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45317AD7-5C30-46D0-872B-DFCD5842CEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29AD50F-35E3-47CD-9AB3-F3FB7A178776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4905" yWindow="1590" windowWidth="21600" windowHeight="11385" xr2:uid="{2B52D150-49A4-4119-BA44-19144FBB2A51}"/>
+    <workbookView xWindow="-27405" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{2B52D150-49A4-4119-BA44-19144FBB2A51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,12 +84,6 @@
     <t>Out</t>
   </si>
   <si>
-    <t>DPRA_pCysDep</t>
-  </si>
-  <si>
-    <t>DPRA_pLysDep</t>
-  </si>
-  <si>
     <t>hCLAT_call</t>
   </si>
   <si>
@@ -105,10 +99,16 @@
     <t>KS_iMax</t>
   </si>
   <si>
-    <t>OECDQSARTB_pred</t>
-  </si>
-  <si>
-    <t>OECDQSARTB_AD</t>
+    <t>inSilico_AD</t>
+  </si>
+  <si>
+    <t>insilico_call</t>
+  </si>
+  <si>
+    <t>DPRA_pC</t>
+  </si>
+  <si>
+    <t>DPRA_pK</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1560DC-E06F-4D73-AE27-83DC3C7B3A02}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -477,31 +479,31 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
         <v>21</v>
-      </c>
-      <c r="H1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add section for comparing results to reference, update UI, clean code
</commit_message>
<xml_diff>
--- a/www/DASSApp-dataTemplate.xlsx
+++ b/www/DASSApp-dataTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kto\Documents\repos\dass\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29AD50F-35E3-47CD-9AB3-F3FB7A178776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142164FD-54CB-4E8B-A163-917E74B0E498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27405" yWindow="3030" windowWidth="21600" windowHeight="11385" xr2:uid="{2B52D150-49A4-4119-BA44-19144FBB2A51}"/>
+    <workbookView xWindow="2475" yWindow="495" windowWidth="21600" windowHeight="14850" xr2:uid="{2B52D150-49A4-4119-BA44-19144FBB2A51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>CASRN</t>
   </si>
@@ -94,9 +94,6 @@
   </si>
   <si>
     <t>KS_call</t>
-  </si>
-  <si>
-    <t>KS_iMax</t>
   </si>
   <si>
     <t>inSilico_AD</t>
@@ -461,11 +458,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1560DC-E06F-4D73-AE27-83DC3C7B3A02}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -474,7 +469,7 @@
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -482,10 +477,10 @@
         <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -497,16 +492,13 @@
         <v>19</v>
       </c>
       <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -529,16 +521,13 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <v>7.6085345990000004</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -561,16 +550,13 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>3.2463792009999999</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -593,16 +579,13 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>1.406772001</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -625,16 +608,13 @@
         <v>1</v>
       </c>
       <c r="H5">
-        <v>18.38</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -657,16 +637,13 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -689,16 +666,13 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1.42</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -718,16 +692,13 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -750,16 +721,13 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>1.3488727149999999</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -781,14 +749,14 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -810,14 +778,14 @@
       <c r="G11">
         <v>0</v>
       </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
       <c r="I11" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -839,14 +807,14 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -868,10 +836,10 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>